<commit_message>
tabs rownames repaired ...
</commit_message>
<xml_diff>
--- a/tabs/crosstabs/frekvence.kataplexií.xlsx
+++ b/tabs/crosstabs/frekvence.kataplexií.xlsx
@@ -14,237 +14,249 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
-  <si>
-    <t xml:space="preserve"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+  <si>
+    <t xml:space="preserve">Issue</t>
   </si>
   <si>
     <t xml:space="preserve">.</t>
   </si>
   <si>
+    <t xml:space="preserve">No time for hobbies due to sleepiness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 (0.00 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forgetting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor-quality night sleep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (0.46 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (1.38 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oversleeping and missing something important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impossibility to sport due to symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fear of motherhood due to symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (0.92 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic behavior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No problem reported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feeling unrefreshed after daytime/nocturnal sleep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems to find the job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nightmares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (1.83 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The necessity to take medication due to symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypnagogic hallucinations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (2.29 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleep paralysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems with concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (2.75 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lack of time spent with children due to symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fear of the disease getting worse in time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 (4.13 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fear of losing the job</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limited work/home performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 (3.21 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cataplexy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 (5.50 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feelings of incompetence (work area)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driving ban/difficulty to drive due to symptoms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 (5.05 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty waking up after a nocturnal sleep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limited social life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stigmatization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feelings of inferiority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 (7.80 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falling asleep in calm situations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 (8.26 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imperative sleepiness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 (11.93 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad mood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 (7.34 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatigue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (9.17 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
-    <t xml:space="preserve">3 (1.38 %)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">16 (7.34 %)</t>
-  </si>
-  <si>
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">12 (5.50 %)</t>
-  </si>
-  <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
-    <t xml:space="preserve">7 (3.21 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (5.05 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 (8.26 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 (9.17 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (2.29 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (0.92 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 (4.13 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 (0.00 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 (7.80 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 (11.93 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (0.46 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (1.83 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (2.75 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
+    <t xml:space="preserve">1 (1.92 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (4.00 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (2.63 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (1.79 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (2.00 %)</t>
   </si>
   <si>
     <t xml:space="preserve">2 (3.57 %)</t>
   </si>
   <si>
-    <t xml:space="preserve">1 (2.00 %)</t>
+    <t xml:space="preserve">3 (5.36 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 (4.55 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (3.85 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (7.89 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (9.09 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (10.71 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (10.00 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (5.26 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (5.77 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (7.14 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (6.00 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (8.00 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (9.62 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (8.93 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (10.53 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (11.54 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 (16.00 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (18.18 %)</t>
   </si>
   <si>
     <t xml:space="preserve">4 (7.69 %)</t>
   </si>
   <si>
-    <t xml:space="preserve">4 (7.14 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (4.00 %)</t>
-  </si>
-  <si>
     <t xml:space="preserve">5 (13.16 %)</t>
   </si>
   <si>
-    <t xml:space="preserve">1 (4.55 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (10.71 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (10.00 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (2.63 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (1.92 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (9.09 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (3.85 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (5.26 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (11.54 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (8.00 %)</t>
-  </si>
-  <si>
     <t xml:space="preserve">8 (15.38 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (6.00 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (10.53 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 (1.79 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (7.89 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (9.62 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (8.93 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (5.36 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 (16.00 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (18.18 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (5.77 %)</t>
   </si>
 </sst>
 </file>
@@ -597,188 +609,188 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
@@ -786,50 +798,50 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
         <v>48</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -854,16 +866,16 @@
         <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -871,19 +883,19 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -891,599 +903,599 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
         <v>76</v>
       </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1508,16 +1520,16 @@
         <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -1525,19 +1537,19 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -1545,599 +1557,599 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F26" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F27" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
         <v>76</v>
       </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
         <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="F32" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>